<commit_message>
delete z which has already been included in alpha
</commit_message>
<xml_diff>
--- a/output/low_rank_high_rank.xlsx
+++ b/output/low_rank_high_rank.xlsx
@@ -453,17 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>optionB; optionB</t>
+          <t>optionB; statement</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -472,17 +472,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>optionB; statement</t>
+          <t>statement; optionB</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -491,17 +491,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>statement; optionB</t>
+          <t>statement; optionD</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="D4" t="n">
-        <v>184</v>
+        <v>93</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -510,17 +510,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>statement; optionB; optionB</t>
+          <t>statement; optionD; optionB</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>193</v>
+        <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -529,17 +529,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>statement; optionB; statement</t>
+          <t>optionD; optionB</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="D6" t="n">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -548,17 +548,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>statement; statement</t>
+          <t>optionD; statement</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="D7" t="n">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -567,17 +567,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>statement; statement; optionB</t>
+          <t>optionA; optionB; statement</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="D8" t="n">
-        <v>216</v>
+        <v>111</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -586,17 +586,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>statement; statement; optionB; optionB</t>
+          <t>optionA; statement; optionB</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>225</v>
+        <v>134</v>
       </c>
       <c r="D9" t="n">
-        <v>217</v>
+        <v>126</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -605,17 +605,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>statement; statement; optionB; statement</t>
+          <t>optionA; optionB</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>226</v>
+        <v>114</v>
       </c>
       <c r="D10" t="n">
-        <v>217</v>
+        <v>105</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -624,17 +624,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>statement; statement; statement</t>
+          <t>optionA; statement</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>229</v>
+        <v>129</v>
       </c>
       <c r="D11" t="n">
-        <v>219</v>
+        <v>119</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -643,17 +643,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>statement; statement; statement; optionB</t>
+          <t>optionA; statement; optionD; optionB</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>231</v>
+        <v>141</v>
       </c>
       <c r="D12" t="n">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -662,17 +662,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>statement; statement; statement; statement</t>
+          <t>optionA; statement; optionD</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>232</v>
+        <v>139</v>
       </c>
       <c r="D13" t="n">
-        <v>220</v>
+        <v>127</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -681,17 +681,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>statement; statement; statement; optionD</t>
+          <t>optionA; optionD; optionB</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>233</v>
+        <v>153</v>
       </c>
       <c r="D14" t="n">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -700,17 +700,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>statement; statement; optionD</t>
+          <t>optionA; optionD; statement</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>235</v>
+        <v>157</v>
       </c>
       <c r="D15" t="n">
-        <v>221</v>
+        <v>143</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -719,17 +719,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>statement; statement; optionD; optionB</t>
+          <t>optionA; optionD</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>237</v>
+        <v>149</v>
       </c>
       <c r="D16" t="n">
-        <v>222</v>
+        <v>134</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -738,17 +738,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>statement; statement; optionD; statement</t>
+          <t>optionA; statement; optionB; diagram</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="D17" t="n">
-        <v>222</v>
+        <v>177</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -757,17 +757,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>statement; optionD</t>
+          <t>statement; optionB; diagram</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>247</v>
+        <v>84</v>
       </c>
       <c r="D18" t="n">
-        <v>230</v>
+        <v>67</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -776,17 +776,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>statement; optionD; optionB</t>
+          <t>optionA; optionB; diagram</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>252</v>
+        <v>115</v>
       </c>
       <c r="D19" t="n">
-        <v>234</v>
+        <v>97</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -795,17 +795,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>statement; optionD; statement</t>
+          <t>optionA; statement; diagram</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>258</v>
+        <v>130</v>
       </c>
       <c r="D20" t="n">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -814,17 +814,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>optionD; optionB</t>
+          <t>optionB; diagram</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>465</v>
+        <v>41</v>
       </c>
       <c r="D21" t="n">
-        <v>445</v>
+        <v>21</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -879,17 +879,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>optionC; optionC</t>
+          <t>optionC; diagram</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>598</v>
+        <v>382</v>
       </c>
       <c r="D2" t="n">
-        <v>597</v>
+        <v>381</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -898,17 +898,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>optionC; optionC; optionC</t>
+          <t>optionC; diagram; statement</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>599</v>
+        <v>672</v>
       </c>
       <c r="D3" t="n">
-        <v>597</v>
+        <v>670</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -917,17 +917,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>optionC; optionC; optionC; optionC</t>
+          <t>optionC; optionB</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>600</v>
+        <v>195</v>
       </c>
       <c r="D4" t="n">
-        <v>597</v>
+        <v>192</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -936,17 +936,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>optionC; optionC; optionC; statement</t>
+          <t>optionC; optionB; diagram</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>762</v>
+        <v>362</v>
       </c>
       <c r="D5" t="n">
-        <v>758</v>
+        <v>358</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -955,17 +955,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>optionC; optionC; optionC; diagram</t>
+          <t>optionC; optionB; diagram; statement</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1176</v>
+        <v>655</v>
       </c>
       <c r="D6" t="n">
-        <v>1171</v>
+        <v>650</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -974,17 +974,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>optionC; optionC; statement</t>
+          <t>optionC; optionB; statement</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>754</v>
+        <v>223</v>
       </c>
       <c r="D7" t="n">
-        <v>748</v>
+        <v>217</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -993,17 +993,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>optionC; optionC; statement; statement</t>
+          <t>optionC; optionB; statement; diagram</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>886</v>
+        <v>337</v>
       </c>
       <c r="D8" t="n">
-        <v>879</v>
+        <v>330</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -1012,17 +1012,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>optionC; optionC; statement; diagram</t>
+          <t>optionC; statement</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>1170</v>
+        <v>196</v>
       </c>
       <c r="D9" t="n">
-        <v>1162</v>
+        <v>188</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -1031,17 +1031,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>optionC; optionC; diagram</t>
+          <t>optionC; statement; diagram</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>1216</v>
+        <v>361</v>
       </c>
       <c r="D10" t="n">
-        <v>1207</v>
+        <v>352</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -1050,17 +1050,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>optionC; optionC; diagram; statement</t>
+          <t>diagram; optionB</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>2358</v>
+        <v>111</v>
       </c>
       <c r="D11" t="n">
-        <v>2348</v>
+        <v>101</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -1069,17 +1069,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>optionC; optionC; diagram; diagram</t>
+          <t>diagram; optionB; statement</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>1352</v>
+        <v>98</v>
       </c>
       <c r="D12" t="n">
-        <v>1341</v>
+        <v>87</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -1088,17 +1088,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>optionC; optionB</t>
+          <t>diagram; optionB; statement; optionC</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>606</v>
+        <v>510</v>
       </c>
       <c r="D13" t="n">
-        <v>594</v>
+        <v>498</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -1107,17 +1107,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionC</t>
+          <t>diagram; optionB; statement; optionD</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>920</v>
+        <v>511</v>
       </c>
       <c r="D14" t="n">
-        <v>907</v>
+        <v>498</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -1126,17 +1126,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionC; optionC</t>
+          <t>diagram; optionB; optionC</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>929</v>
+        <v>545</v>
       </c>
       <c r="D15" t="n">
-        <v>915</v>
+        <v>531</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -1145,17 +1145,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionC; statement</t>
+          <t>diagram; optionB; optionC; statement</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>914</v>
+        <v>466</v>
       </c>
       <c r="D16" t="n">
-        <v>899</v>
+        <v>451</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -1164,17 +1164,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionC; diagram</t>
+          <t>diagram; optionB; optionD</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>1173</v>
+        <v>546</v>
       </c>
       <c r="D17" t="n">
-        <v>1157</v>
+        <v>530</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -1183,17 +1183,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionB</t>
+          <t>diagram; optionB; optionD; optionC</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>607</v>
+        <v>870</v>
       </c>
       <c r="D18" t="n">
-        <v>590</v>
+        <v>853</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -1202,17 +1202,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionB; optionC</t>
+          <t>diagram; optionB; optionD; statement</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>976</v>
+        <v>876</v>
       </c>
       <c r="D19" t="n">
-        <v>958</v>
+        <v>858</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -1221,17 +1221,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionB; statement</t>
+          <t>diagram; statement</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>761</v>
+        <v>110</v>
       </c>
       <c r="D20" t="n">
-        <v>742</v>
+        <v>91</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -1240,17 +1240,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>optionC; optionB; optionB; diagram</t>
+          <t>diagram; statement; optionB</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>1039</v>
+        <v>103</v>
       </c>
       <c r="D21" t="n">
-        <v>1019</v>
+        <v>83</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>

</xml_diff>